<commit_message>
Diameter up to 1299 mm, Published
</commit_message>
<xml_diff>
--- a/Screw-conveyor/Example broken screw/Conveyor data.xlsx
+++ b/Screw-conveyor/Example broken screw/Conveyor data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\VTK-Screw-conveyor3\Screw-conveyor\Example broken screw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E38A87-C846-418C-AADB-623813D530D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16577DC5-A4CE-45F5-BC16-1BD8E9F7A0F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10125" yWindow="2580" windowWidth="15855" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="3045" windowWidth="15855" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -176,6 +176,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -462,7 +465,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +628,7 @@
       <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="5">
         <v>70</v>
       </c>
       <c r="C18" t="s">

</xml_diff>

<commit_message>
Bugfix DGV1 line 8 is pipe diameter NOT montage
</commit_message>
<xml_diff>
--- a/Screw-conveyor/Example broken screw/Conveyor data.xlsx
+++ b/Screw-conveyor/Example broken screw/Conveyor data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\VTK-Screw-conveyor3\Screw-conveyor\Example broken screw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16577DC5-A4CE-45F5-BC16-1BD8E9F7A0F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E54297-09F7-4AC1-9181-09343EA845F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="3045" windowWidth="15855" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="780" windowWidth="20685" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Diameter</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Deflection</t>
+  </si>
+  <si>
+    <t>Broken screw after 9 years</t>
   </si>
 </sst>
 </file>
@@ -465,7 +468,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D20" sqref="A1:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,6 +487,11 @@
         <v>44216</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>

</xml_diff>